<commit_message>
Fix BUG Timed sendig data, Task4NextWeek :T4NW:
+ missing break statement in the every case
+ New BUG: :-1:   :ambulance:
 timer.send(msTime) - this method does not adhere to msTime value. The sending of datas is too fast. {to fast /so fast/

Task for this week:
 + After manual initialization the device is stand by bus.off statement. The repeatedly is receiving this commands : "\x0F\t\x02\x02\x02" :alarm_clock:
     - Solve it and succesfully initialize the device.
    - Rewrite broke constans in the automatized #init CMD
 + To reache the communication between the USB2CAN converter
 + Preformating the received data to textBox readable ASCII datas
----------------------------------------------------
 + Code & Decode data for the BLDC motor
       - Use for this HexCommandGenerator + CMD Worspace for clear copy the generated excel command to the ownGUI.

:+1: :+1: :+1:
:alien:
</commit_message>
<xml_diff>
--- a/Additional tools/HexCommandGenerator.xlsx
+++ b/Additional tools/HexCommandGenerator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RPlsicik\Documents\GitHub\RVC\Additional tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6B7A96-E84F-4EBE-8F3F-3106BA8AB908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE58E970-3673-4CD6-B8DB-F39631348BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{C0407B85-B327-42D9-9F5E-F62690023138}"/>
+    <workbookView xWindow="-28920" yWindow="-3720" windowWidth="29040" windowHeight="15840" xr2:uid="{C0407B85-B327-42D9-9F5E-F62690023138}"/>
   </bookViews>
   <sheets>
     <sheet name="CommandGenerator" sheetId="1" r:id="rId1"/>
@@ -1395,8 +1395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC89998-441A-4609-87CE-6352FEC4F125}">
   <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F10" sqref="F9:V10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3034,13 +3034,13 @@
       </c>
       <c r="B51" s="37" t="str">
         <f t="shared" si="4"/>
-        <v>x0fx13x02x04x03</v>
+        <v>x0fx04x02x04x03</v>
       </c>
       <c r="C51" s="38" t="s">
         <v>0</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="E51" s="39" t="str">
         <f t="shared" ref="E51" si="8">"x0"&amp;DEC2HEX(COLUMNS(F51:T51)-COUNTBLANK(F51:T51))</f>
@@ -3251,7 +3251,7 @@
   <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3263,30 +3263,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B2" s="8"/>
@@ -3644,6 +3644,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4148,7 +4149,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4506,8 +4507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A5977F-5E27-47AA-A937-D45A32611ECA}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>